<commit_message>
adding ch4/nh3 data files
</commit_message>
<xml_diff>
--- a/resources/input/stagnation/CH4_NH3/20%_data_reduced.xlsx
+++ b/resources/input/stagnation/CH4_NH3/20%_data_reduced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marina/Developer/transport-spherical/resources/input/stagnation/CH4_NH3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034C9357-9963-454F-A365-56EBAF57DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092FBB67-9ED2-BE4B-9635-E19CFF3DDB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{3EE0DCB7-C210-924A-A5DE-691BF3640D7B}"/>
   </bookViews>
@@ -244,10 +244,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,9 +274,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -279,9 +295,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,1044 +320,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$AY$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AK$2:$AK$109</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="108"/>
-                <c:pt idx="0">
-                  <c:v>0.6498739604999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.69953301175000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.74994001124999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.79992299249999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.84934796975000015</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.89929078350000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.94941619374999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.99796388925000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0485257100000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0994189194999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.1488364530000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.19940770425</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2492147843333334</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.2994637849999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.3500328457499999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.398869897</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.94621072900000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AY$2:$AY$109</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="108"/>
-                <c:pt idx="0">
-                  <c:v>4699.8264240000008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5831.522919</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6676.7746312500003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7329.4831555000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7429.6770592499997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7762.6486080000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7907.5266257499998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7719.9142365000007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7191.4039777500002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6509.79075775</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5559.4415214999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4293.0194217500002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2504.767018</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>104.35420887000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25.3783567075</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-8.6834776695000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8033.8468159999993</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7879.9897424999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-87A0-3244-B30D-290D6E783C55}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1949461552"/>
-        <c:axId val="2129110367"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1949461552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.4"/>
-          <c:min val="0.4"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2129110367"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2129110367"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1949461552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>726205</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>158343</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>340641</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>149877</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C06D2E1-35B9-A518-464D-93410F8D2C82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1636,13 +621,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB62E82B-E963-9340-876F-AC0E4B8CA7C2}">
   <dimension ref="A1:BR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="BR2" sqref="AI2:BR12"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="BG39" sqref="BG39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="34" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="34" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.2">
@@ -5487,7 +4472,7 @@
         <f ca="1">SQRT((AVERAGE(OFFSET(T$3,((ROW(T14)-1)*4)+1,0):OFFSET(T$3,((ROW(T14))*4),0))^2)+(STDEV(OFFSET(S$3,((ROW(S14)-1)*4)+1,0):OFFSET(S$3,((ROW(S14))*4),0)))^2)</f>
         <v>28.135713171343557</v>
       </c>
-      <c r="BE16">
+      <c r="BE16" s="1">
         <f ca="1">AVERAGE(OFFSET(U$3,((ROW(U14)-1)*4)+1,0):OFFSET(U$3,((ROW(U14))*4),0))</f>
         <v>3142.7519417499998</v>
       </c>
@@ -5503,7 +4488,7 @@
         <f ca="1">SQRT((AVERAGE(OFFSET(X$3,((ROW(X14)-1)*4)+1,0):OFFSET(X$3,((ROW(X14))*4),0))^2)+(STDEV(OFFSET(W$3,((ROW(W14)-1)*4)+1,0):OFFSET(W$3,((ROW(W14))*4),0)))^2)</f>
         <v>14.226820726753022</v>
       </c>
-      <c r="BI16">
+      <c r="BI16" s="1">
         <f ca="1">AVERAGE(OFFSET(Y$3,((ROW(Y14)-1)*4)+1,0):OFFSET(Y$3,((ROW(Y14))*4),0))</f>
         <v>3325.9598660000001</v>
       </c>
@@ -5733,7 +4718,7 @@
         <f ca="1">SQRT((AVERAGE(OFFSET(T$3,((ROW(T15)-1)*4)+1,0):OFFSET(T$3,((ROW(T15))*4),0))^2)+(STDEV(OFFSET(S$3,((ROW(S15)-1)*4)+1,0):OFFSET(S$3,((ROW(S15))*4),0)))^2)</f>
         <v>358.37437293868203</v>
       </c>
-      <c r="BE17">
+      <c r="BE17" s="1">
         <f ca="1">AVERAGE(OFFSET(U$3,((ROW(U15)-1)*4)+1,0):OFFSET(U$3,((ROW(U15))*4),0))</f>
         <v>7386.4143125000001</v>
       </c>
@@ -5749,7 +4734,7 @@
         <f ca="1">SQRT((AVERAGE(OFFSET(X$3,((ROW(X15)-1)*4)+1,0):OFFSET(X$3,((ROW(X15))*4),0))^2)+(STDEV(OFFSET(W$3,((ROW(W15)-1)*4)+1,0):OFFSET(W$3,((ROW(W15))*4),0)))^2)</f>
         <v>218.55358386871185</v>
       </c>
-      <c r="BI17">
+      <c r="BI17" s="1">
         <f ca="1">AVERAGE(OFFSET(Y$3,((ROW(Y15)-1)*4)+1,0):OFFSET(Y$3,((ROW(Y15))*4),0))</f>
         <v>10216.944879999999</v>
       </c>
@@ -8047,6 +7032,8 @@
       <c r="AH28">
         <v>0.46599102999999997</v>
       </c>
+      <c r="BH28" s="3"/>
+      <c r="BI28" s="3"/>
     </row>
     <row r="29" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -8151,6 +7138,8 @@
       <c r="AH29">
         <v>0.46519445999999998</v>
       </c>
+      <c r="BH29" s="3"/>
+      <c r="BI29" s="3"/>
     </row>
     <row r="30" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -8255,6 +7244,8 @@
       <c r="AH30">
         <v>0.452098108</v>
       </c>
+      <c r="BH30" s="3"/>
+      <c r="BI30" s="4"/>
     </row>
     <row r="31" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -8359,6 +7350,8 @@
       <c r="AH31">
         <v>0.45119605699999998</v>
       </c>
+      <c r="BH31" s="3"/>
+      <c r="BI31" s="4"/>
     </row>
     <row r="32" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -8463,8 +7456,10 @@
       <c r="AH32">
         <v>0.42638351600000002</v>
       </c>
+      <c r="BH32" s="3"/>
+      <c r="BI32" s="4"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8567,8 +7562,10 @@
       <c r="AH33">
         <v>0.46564588299999998</v>
       </c>
+      <c r="BH33" s="3"/>
+      <c r="BI33" s="4"/>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8671,8 +7668,12 @@
       <c r="AH34">
         <v>0.42646033</v>
       </c>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="BH34" s="3"/>
+      <c r="BI34" s="4"/>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8775,8 +7776,12 @@
       <c r="AH35">
         <v>0.42679719700000002</v>
       </c>
+      <c r="AQ35" s="2"/>
+      <c r="AR35" s="2"/>
+      <c r="BH35" s="3"/>
+      <c r="BI35" s="4"/>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>37</v>
       </c>
@@ -8879,8 +7884,12 @@
       <c r="AH36">
         <v>0.469537912</v>
       </c>
+      <c r="AQ36" s="2"/>
+      <c r="AR36" s="2"/>
+      <c r="BH36" s="3"/>
+      <c r="BI36" s="4"/>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>38</v>
       </c>
@@ -8983,8 +7992,12 @@
       <c r="AH37">
         <v>0.42602610299999999</v>
       </c>
+      <c r="AQ37" s="2"/>
+      <c r="AR37" s="2"/>
+      <c r="BH37" s="3"/>
+      <c r="BI37" s="4"/>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>39</v>
       </c>
@@ -9087,8 +8100,12 @@
       <c r="AH38">
         <v>0.46888996399999999</v>
       </c>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="2"/>
+      <c r="BH38" s="3"/>
+      <c r="BI38" s="4"/>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>40</v>
       </c>
@@ -9191,8 +8208,12 @@
       <c r="AH39">
         <v>0.42514763100000003</v>
       </c>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="2"/>
+      <c r="BH39" s="3"/>
+      <c r="BI39" s="4"/>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>41</v>
       </c>
@@ -9295,8 +8316,12 @@
       <c r="AH40">
         <v>0.46678273999999997</v>
       </c>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="2"/>
+      <c r="BH40" s="3"/>
+      <c r="BI40" s="4"/>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>42</v>
       </c>
@@ -9399,8 +8424,12 @@
       <c r="AH41">
         <v>0.46671184399999999</v>
       </c>
+      <c r="AQ41" s="2"/>
+      <c r="AR41" s="2"/>
+      <c r="BH41" s="3"/>
+      <c r="BI41" s="4"/>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>43</v>
       </c>
@@ -9503,8 +8532,12 @@
       <c r="AH42">
         <v>0.406428864</v>
       </c>
+      <c r="AQ42" s="2"/>
+      <c r="AR42" s="2"/>
+      <c r="BH42" s="3"/>
+      <c r="BI42" s="4"/>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>44</v>
       </c>
@@ -9607,8 +8640,12 @@
       <c r="AH43">
         <v>0.40559133600000002</v>
       </c>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2"/>
+      <c r="BH43" s="3"/>
+      <c r="BI43" s="3"/>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>45</v>
       </c>
@@ -9711,8 +8748,10 @@
       <c r="AH44">
         <v>0.46589837000000001</v>
       </c>
+      <c r="AQ44" s="2"/>
+      <c r="AR44" s="2"/>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>46</v>
       </c>
@@ -9815,8 +8854,10 @@
       <c r="AH45">
         <v>0.35866130000000002</v>
       </c>
+      <c r="AQ45" s="2"/>
+      <c r="AR45" s="2"/>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>47</v>
       </c>
@@ -9919,8 +8960,10 @@
       <c r="AH46">
         <v>0.46533383499999997</v>
       </c>
+      <c r="AQ46" s="2"/>
+      <c r="AR46" s="2"/>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>48</v>
       </c>
@@ -10024,7 +9067,7 @@
         <v>0.35846814199999999</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>49</v>
       </c>
@@ -11378,7 +10421,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>